<commit_message>
Update `get_level_from_xp.xlsx` with all attributes
</commit_message>
<xml_diff>
--- a/get_level_from_xp.xlsx
+++ b/get_level_from_xp.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28816"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\AppData\Local\Temp\fz3temp-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE16172-040E-41E9-BA33-0A92F6E67DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA1A49B-611A-407F-80E8-0B17DDA0CCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3391A42-EC4B-4A2C-93AB-0FF5C027C8D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{B3391A42-EC4B-4A2C-93AB-0FF5C027C8D0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="defense" sheetId="2" r:id="rId1"/>
+    <sheet name="max_health" sheetId="3" r:id="rId2"/>
+    <sheet name="speed" sheetId="4" r:id="rId3"/>
+    <sheet name="strength" sheetId="5" r:id="rId4"/>
+    <sheet name="get_level_from_xp" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>rpg_lvl_defense</t>
+  </si>
+  <si>
+    <t>generic.armor</t>
+  </si>
+  <si>
+    <t>rpg_lvl_max_health</t>
+  </si>
+  <si>
+    <t>generic.max_health</t>
+  </si>
+  <si>
+    <t>rpg_lvl_speed</t>
+  </si>
+  <si>
+    <t>generic.movement_speed</t>
+  </si>
+  <si>
+    <t>rpg_lvl_strength</t>
+  </si>
+  <si>
+    <t>generic.attack_damage</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,6 +434,1414 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D13C4D-7C9F-47AC-863A-D6E425CA3739}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>C1</f>
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"execute if score @s " &amp; $A$1 &amp; " matches " &amp; B2 &amp; " run attribute @s " &amp; $B$1 &amp; " modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats " &amp; C2 &amp; " add"</f>
+        <v>execute if score @s rpg_lvl_defense matches 1 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 1 add</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>C2+$C$1</f>
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D26" si="0">"execute if score @s " &amp; $A$1 &amp; " matches " &amp; B3 &amp; " run attribute @s " &amp; $B$1 &amp; " modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats " &amp; C3 &amp; " add"</f>
+        <v>execute if score @s rpg_lvl_defense matches 2 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 2 add</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="1">C3+$C$1</f>
+        <v>3</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 3 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 3 add</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 4 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 4 add</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 5 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 5 add</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 6 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 6 add</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 7 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 7 add</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 8 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 8 add</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 9 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 9 add</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 10 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 10 add</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 11 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 11 add</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 12 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 12 add</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 13 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 13 add</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 14 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 14 add</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 15 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 15 add</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 16 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 16 add</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 17 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 17 add</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 18 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 18 add</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 19 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 19 add</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 20 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 20 add</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 21 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 21 add</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 22 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 22 add</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 23 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 23 add</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 24 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 24 add</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_defense matches 25 run attribute @s generic.armor modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 25 add</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F99DDA-8710-401A-81E6-2DC6A043C594}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>C1</f>
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"execute if score @s " &amp; $A$1 &amp; " matches " &amp; B2 &amp; " run attribute @s " &amp; $B$1 &amp; " modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats " &amp; C2 &amp; " add"</f>
+        <v>execute if score @s rpg_lvl_max_health matches 1 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 1 add</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>C2+$C$1</f>
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D26" si="0">"execute if score @s " &amp; $A$1 &amp; " matches " &amp; B3 &amp; " run attribute @s " &amp; $B$1 &amp; " modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats " &amp; C3 &amp; " add"</f>
+        <v>execute if score @s rpg_lvl_max_health matches 2 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 2 add</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="1">C3+$C$1</f>
+        <v>3</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 3 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 3 add</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 4 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 4 add</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 5 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 5 add</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 6 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 6 add</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 7 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 7 add</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 8 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 8 add</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 9 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 9 add</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 10 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 10 add</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 11 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 11 add</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 12 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 12 add</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 13 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 13 add</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 14 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 14 add</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 15 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 15 add</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 16 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 16 add</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 17 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 17 add</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 18 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 18 add</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 19 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 19 add</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 20 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 20 add</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 21 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 21 add</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 22 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 22 add</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 23 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 23 add</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 24 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 24 add</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_max_health matches 25 run attribute @s generic.max_health modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 25 add</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622B69B1-F4F8-458C-A04C-B7378FF32516}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>C1</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"execute if score @s " &amp; $A$1 &amp; " matches " &amp; B2 &amp; " run attribute @s " &amp; $B$1 &amp; " modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats " &amp; SUBSTITUTE(C2,",",".") &amp; " add"</f>
+        <v>execute if score @s rpg_lvl_speed matches 1 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.003 add</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>C2+$C$1</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D26" si="0">"execute if score @s " &amp; $A$1 &amp; " matches " &amp; B3 &amp; " run attribute @s " &amp; $B$1 &amp; " modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats " &amp; SUBSTITUTE(C3,",",".") &amp; " add"</f>
+        <v>execute if score @s rpg_lvl_speed matches 2 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.006 add</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="1">C3+$C$1</f>
+        <v>9.0000000000000011E-3</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 3 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.009 add</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>1.2E-2</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 4 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.012 add</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 5 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.015 add</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 6 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.018 add</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>2.0999999999999998E-2</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 7 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.021 add</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>2.3999999999999997E-2</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 8 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.024 add</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>2.6999999999999996E-2</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 9 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.027 add</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>2.9999999999999995E-2</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 10 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.03 add</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>3.2999999999999995E-2</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 11 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.033 add</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 12 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.036 add</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>3.9E-2</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 13 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.039 add</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 14 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.042 add</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 15 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.045 add</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>4.8000000000000008E-2</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 16 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.048 add</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>5.1000000000000011E-2</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 17 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.051 add</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>5.4000000000000013E-2</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 18 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.054 add</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>5.7000000000000016E-2</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 19 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.057 add</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000019E-2</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 20 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.06 add</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>6.3000000000000014E-2</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 21 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.063 add</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>6.6000000000000017E-2</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 22 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.066 add</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>6.900000000000002E-2</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 23 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.069 add</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>7.2000000000000022E-2</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 24 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.072 add</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>7.5000000000000025E-2</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_speed matches 25 run attribute @s generic.movement_speed modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.075 add</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF8125A-406F-4B23-AD8B-797387BB233C}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>C1</f>
+        <v>0.01</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"execute if score @s " &amp; $A$1 &amp; " matches " &amp; B2 &amp; " run attribute @s " &amp; $B$1 &amp; " modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats " &amp; SUBSTITUTE(C2,",",".") &amp; " add"</f>
+        <v>execute if score @s rpg_lvl_strength matches 1 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.01 add</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>C2+$C$1</f>
+        <v>0.02</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D26" si="0">"execute if score @s " &amp; $A$1 &amp; " matches " &amp; B3 &amp; " run attribute @s " &amp; $B$1 &amp; " modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats " &amp; SUBSTITUTE(C3,",",".") &amp; " add"</f>
+        <v>execute if score @s rpg_lvl_strength matches 2 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.02 add</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="1">C3+$C$1</f>
+        <v>0.03</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 3 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.03 add</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 4 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.04 add</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 5 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.05 add</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 6 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.06 add</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 7 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.07 add</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 8 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.08 add</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 9 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.09 add</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 10 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.1 add</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 11 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.11 add</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 12 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.12 add</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0.12999999999999998</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 13 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.13 add</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 14 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.14 add</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 15 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.15 add</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.16</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 16 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.16 add</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0.17</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 17 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.17 add</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>0.18000000000000002</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 18 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.18 add</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>0.19000000000000003</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 19 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.19 add</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 20 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.2 add</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>0.21000000000000005</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 21 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.21 add</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>0.22000000000000006</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 22 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.22 add</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>0.23000000000000007</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 23 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.23 add</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>0.24000000000000007</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 24 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.24 add</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>execute if score @s rpg_lvl_strength matches 25 run attribute @s generic.attack_damage modifier add 891dde02-2eec-45eb-8b4a-a68f3b0acc7a rpg_stats 0.25 add</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482E0771-2BA8-44E3-A134-66FD6CB1651A}">
   <dimension ref="A1:D100"/>
   <sheetViews>

</xml_diff>